<commit_message>
Added shuffle button and updated background
</commit_message>
<xml_diff>
--- a/vocab/tocfl_1.xlsx
+++ b/vocab/tocfl_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\Files\python_work\scripts_for_fun\chinese_flashcards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\Files\javascript\chinese_flashcards\vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58600E45-0617-4CC9-B109-FCB8A1F19888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7BB7DF-1234-4EBE-AA2D-9D044F8E69DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4537,7 +4537,7 @@
   <dimension ref="A1:F304"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191"/>
+      <selection activeCell="B2" sqref="A2:XFD301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>